<commit_message>
03. 08. - 11:42
</commit_message>
<xml_diff>
--- a/CCC/Homeworks/Adam_Ancsin_homework1.xlsx
+++ b/CCC/Homeworks/Adam_Ancsin_homework1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">SHORTLIST OF SELECTED U.S. HIGHER EDUCATION INSTITUTIONS</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t xml:space="preserve">High rate of financial aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I see these goals are quite ambitious. However, I would like to stress that aiming for a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">high prestige schhol is crucial for me to achievie my highest performance and I would </t>
+  </si>
+  <si>
+    <t xml:space="preserve">not like to settle for less.</t>
   </si>
 </sst>
 </file>
@@ -161,9 +173,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -286,85 +297,69 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -616,199 +611,235 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -824,6 +855,10 @@
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
03. 09. - 16:11
</commit_message>
<xml_diff>
--- a/CCC/Homeworks/Adam_Ancsin_homework1.xlsx
+++ b/CCC/Homeworks/Adam_Ancsin_homework1.xlsx
@@ -103,10 +103,10 @@
     <t xml:space="preserve">Note:</t>
   </si>
   <si>
-    <t xml:space="preserve">I see these goals are quite ambitious. However, I would like to stress that aiming for a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">high prestige schhol is crucial for me to achievie my highest performance and I would </t>
+    <t xml:space="preserve">I see these goals are quite ambitious. However, I would like to stress that aiming for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">high prestige schools is crucial for me to achievie my highest performance and I would </t>
   </si>
   <si>
     <t xml:space="preserve">not like to settle for less.</t>
@@ -119,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,12 +172,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -297,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,7 +352,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -613,8 +611,8 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -834,9 +832,11 @@
       <c r="E20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>